<commit_message>
Updated gitignore, removed excel temporary file
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5722AE6F-F81D-4EC3-AC52-FC9FF86A0387}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053FED49-8ED6-46B8-B88B-82EBB3070771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19155" yWindow="585" windowWidth="19080" windowHeight="13860" tabRatio="729" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2931,13 +2931,13 @@
   <dimension ref="A1:I21"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="2" max="2" width="20.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="29.25" style="1" customWidth="1"/>
     <col min="3" max="3" width="6.625" customWidth="1"/>
     <col min="5" max="8" width="9.125" customWidth="1"/>
     <col min="9" max="9" width="10.875" style="6"/>
@@ -3161,7 +3161,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
       <c r="B17" s="1" t="s">
         <v>37</v>
       </c>
@@ -3184,7 +3184,7 @@
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3329,7 +3329,7 @@
   <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="D43" sqref="A1:D43"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates after sprint 1, and sprint 2 planning meeting
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053FED49-8ED6-46B8-B88B-82EBB3070771}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CEC31E-4517-49CF-B796-6C7B10A92F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19155" yWindow="585" windowWidth="19080" windowHeight="13860" tabRatio="729" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3975" yWindow="1170" windowWidth="15825" windowHeight="10965" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -28,6 +28,13 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
     </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -36,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="352" uniqueCount="203">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="204">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -142,10 +149,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>hm</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Story ID</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -158,10 +161,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>Done</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>Sprint</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -181,15 +180,6 @@
     <t>GitHub Repository:</t>
   </si>
   <si>
-    <t>Bring pizza to our meetings</t>
-  </si>
-  <si>
-    <t>Leaving leftover pizza on the counter</t>
-  </si>
-  <si>
-    <t>Bring silverware for everyone</t>
-  </si>
-  <si>
     <t>Dates (birth, marriage, divorce, death) should not be after the current date</t>
   </si>
   <si>
@@ -677,6 +667,24 @@
   </si>
   <si>
     <t>???</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Working separately but at the same time</t>
+  </si>
+  <si>
+    <t>Working together, asking eachother how they're doing it (reduces duplicate code)</t>
+  </si>
+  <si>
+    <t>Doing work that’s already included in another user story</t>
+  </si>
+  <si>
+    <t>Pushing code with syntax errors that doesn't compile; not testing your code before pushing.</t>
+  </si>
+  <si>
+    <t>Helping eachother with dev environment setup</t>
   </si>
 </sst>
 </file>
@@ -819,7 +827,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -857,6 +865,8 @@
     <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="66">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1106,10 +1116,10 @@
                 <c:formatCode>m/d</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>40442</c:v>
+                  <c:v>43011</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>40455</c:v>
+                  <c:v>43025</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1121,10 +1131,10 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>36</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>30</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1238,15 +1248,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>469053</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>25401</xdr:rowOff>
+      <xdr:colOff>231913</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>115956</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
       <xdr:colOff>948266</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>160867</xdr:rowOff>
+      <xdr:rowOff>160866</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1261,8 +1271,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1425786" y="533401"/>
-          <a:ext cx="1317413" cy="643466"/>
+          <a:off x="1060174" y="1441173"/>
+          <a:ext cx="1436940" cy="707519"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -1517,15 +1527,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>20320</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:colOff>20319</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>157371</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>1100666</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>149086</xdr:colOff>
       <xdr:row>12</xdr:row>
-      <xdr:rowOff>101599</xdr:rowOff>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -1540,8 +1550,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4930987" y="1371600"/>
-          <a:ext cx="1080346" cy="761999"/>
+          <a:off x="4244449" y="1151284"/>
+          <a:ext cx="1081267" cy="938142"/>
         </a:xfrm>
         <a:prstGeom prst="wedgeRectCallout">
           <a:avLst>
@@ -2015,7 +2025,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A6"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2040,83 +2050,83 @@
         <v>22</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C3" t="s">
         <v>181</v>
       </c>
-      <c r="B3" t="s">
-        <v>185</v>
-      </c>
-      <c r="C3" t="s">
-        <v>186</v>
-      </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E3" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" t="s">
         <v>182</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
+        <v>183</v>
+      </c>
+      <c r="D4" t="s">
         <v>187</v>
       </c>
-      <c r="C4" t="s">
-        <v>188</v>
-      </c>
-      <c r="D4" t="s">
-        <v>192</v>
-      </c>
       <c r="E4" s="17" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="B5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="C5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="D5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="B6" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="C6" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="D6" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="D9" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E9" s="16" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
     </row>
   </sheetData>
@@ -2136,8 +2146,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2151,19 +2161,19 @@
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C1" s="4" t="s">
         <v>18</v>
       </c>
       <c r="D1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="4" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
@@ -2171,133 +2181,149 @@
         <v>1</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="C2" s="19" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="D2" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E2" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="E2" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="19" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="C3" s="19" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="D3" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="E3" s="19"/>
+        <v>178</v>
+      </c>
+      <c r="E3" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C4" s="19" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="D4" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E4" s="19"/>
+        <v>177</v>
+      </c>
+      <c r="E4" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D5" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="E5" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="E5" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="D6" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E6" s="19"/>
+        <v>178</v>
+      </c>
+      <c r="E6" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="C7" s="19" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="D7" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="E7" s="19"/>
+        <v>177</v>
+      </c>
+      <c r="E7" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="D8" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="E8" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="E8" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="C9" s="19" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="D9" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="E9" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="E9" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
       <c r="B10" s="19" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="C10" s="19" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="D10" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E10" s="19"/>
     </row>
@@ -2306,13 +2332,13 @@
         <v>2</v>
       </c>
       <c r="B11" s="19" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="C11" s="19" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D11" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E11" s="19"/>
     </row>
@@ -2321,13 +2347,13 @@
         <v>2</v>
       </c>
       <c r="B12" s="19" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="C12" s="19" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D12" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E12" s="19"/>
     </row>
@@ -2336,13 +2362,13 @@
         <v>2</v>
       </c>
       <c r="B13" s="19" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="C13" s="19" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="D13" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E13" s="19"/>
     </row>
@@ -2351,13 +2377,13 @@
         <v>2</v>
       </c>
       <c r="B14" s="19" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="C14" s="19" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="D14" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E14" s="19"/>
     </row>
@@ -2366,13 +2392,13 @@
         <v>2</v>
       </c>
       <c r="B15" s="19" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="C15" s="19" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="D15" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E15" s="19"/>
     </row>
@@ -2381,13 +2407,13 @@
         <v>2</v>
       </c>
       <c r="B16" s="19" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="C16" s="19" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="D16" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E16" s="19"/>
     </row>
@@ -2396,13 +2422,13 @@
         <v>2</v>
       </c>
       <c r="B17" s="19" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="C17" s="19" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E17" s="19"/>
     </row>
@@ -2411,13 +2437,13 @@
         <v>3</v>
       </c>
       <c r="B18" s="19" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="C18" s="19" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E18" s="19"/>
     </row>
@@ -2426,13 +2452,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="C19" s="19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E19" s="19"/>
     </row>
@@ -2441,13 +2467,13 @@
         <v>3</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C20" s="19" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E20" s="19"/>
     </row>
@@ -2456,13 +2482,13 @@
         <v>3</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="C21" s="19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E21" s="19"/>
     </row>
@@ -2471,13 +2497,13 @@
         <v>3</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E22" s="19"/>
     </row>
@@ -2486,13 +2512,13 @@
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E23" s="19"/>
     </row>
@@ -2501,13 +2527,13 @@
         <v>3</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E24" s="19"/>
     </row>
@@ -2516,13 +2542,13 @@
         <v>3</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E25" s="19"/>
     </row>
@@ -2531,13 +2557,13 @@
         <v>4</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E26" s="19"/>
     </row>
@@ -2546,13 +2572,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -2561,13 +2587,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E28" s="19"/>
     </row>
@@ -2576,13 +2602,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E29" s="19"/>
     </row>
@@ -2591,13 +2617,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E30" s="19"/>
     </row>
@@ -2606,13 +2632,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E31" s="19"/>
     </row>
@@ -2621,13 +2647,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E32" s="19"/>
     </row>
@@ -2636,13 +2662,13 @@
         <v>4</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E33" s="19"/>
     </row>
@@ -2657,14 +2683,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K38" sqref="K38"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="9.5" customWidth="1"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
     <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.375" customWidth="1"/>
     <col min="5" max="5" width="6.875" customWidth="1"/>
@@ -2673,37 +2699,37 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" s="7" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" s="7" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A5" s="7" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" s="7" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
     </row>
     <row r="14" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>0</v>
@@ -2726,7 +2752,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="B15" s="13">
         <v>41065</v>
@@ -2742,7 +2768,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="B16" s="13">
         <v>41078</v>
@@ -2767,7 +2793,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" s="7" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="B17" s="13">
         <v>41092</v>
@@ -2792,7 +2818,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="7" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="B18" s="13">
         <v>41106</v>
@@ -2817,7 +2843,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="B19" s="13">
         <v>41120</v>
@@ -2852,7 +2878,7 @@
   <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2887,35 +2913,37 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
-        <v>40442</v>
+        <v>43011</v>
       </c>
       <c r="B2">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="D2">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="2">
-        <v>40455</v>
+      <c r="A3" s="7">
+        <v>43025</v>
       </c>
       <c r="B3">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3">
         <f>B2-B3</f>
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="D3">
-        <v>250</v>
+        <f>SUM(Sprint1!G:G)</f>
+        <v>93</v>
       </c>
       <c r="E3">
-        <v>120</v>
+        <f>SUM(Sprint1!H:H)</f>
+        <v>101</v>
       </c>
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
-        <v>125.00000000000001</v>
+        <v>55.24752475247525</v>
       </c>
     </row>
   </sheetData>
@@ -2928,10 +2956,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2972,214 +3000,920 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>121</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="C2" t="s">
-        <v>26</v>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>114</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>156</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>176</v>
       </c>
       <c r="D2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E2">
+        <v>80</v>
+      </c>
+      <c r="F2">
+        <v>12</v>
+      </c>
+      <c r="G2">
+        <v>18</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+      <c r="I2" s="6">
+        <v>43011</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>115</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>69</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" t="s">
+        <v>198</v>
+      </c>
+      <c r="E3">
         <v>30</v>
       </c>
-      <c r="E2">
-        <v>150</v>
-      </c>
-      <c r="F2">
-        <v>60</v>
-      </c>
-      <c r="G2">
-        <v>120</v>
-      </c>
-      <c r="H2">
-        <v>90</v>
-      </c>
-      <c r="I2" s="6">
-        <v>40444</v>
+      <c r="F3">
+        <v>35</v>
+      </c>
+      <c r="G3">
+        <v>13</v>
+      </c>
+      <c r="H3">
+        <v>14</v>
+      </c>
+      <c r="I3" s="6">
+        <v>43011</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B4" s="19" t="s">
-        <v>161</v>
+        <v>68</v>
       </c>
       <c r="C4" s="20" t="s">
-        <v>181</v>
+        <v>177</v>
+      </c>
+      <c r="D4" t="s">
+        <v>198</v>
       </c>
       <c r="E4">
-        <v>80</v>
+        <v>20</v>
       </c>
       <c r="F4">
+        <v>20</v>
+      </c>
+      <c r="G4">
+        <v>8</v>
+      </c>
+      <c r="H4">
         <v>12</v>
+      </c>
+      <c r="I4" s="7">
+        <v>43011</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B5" s="19" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="C5" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="20"/>
+        <v>179</v>
+      </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
       <c r="E5">
-        <v>30</v>
+        <v>15</v>
       </c>
       <c r="F5">
-        <v>35</v>
+        <v>10</v>
+      </c>
+      <c r="G5">
+        <v>6</v>
+      </c>
+      <c r="H5">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7">
+        <v>43011</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B6" s="19" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C6" s="20" t="s">
-        <v>182</v>
+        <v>178</v>
+      </c>
+      <c r="D6" t="s">
+        <v>198</v>
       </c>
       <c r="E6">
         <v>20</v>
       </c>
       <c r="F6">
-        <v>20</v>
+        <v>30</v>
+      </c>
+      <c r="G6">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6" s="7">
+        <v>43011</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="B7" s="19" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="C7" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D7" s="20"/>
+        <v>177</v>
+      </c>
+      <c r="D7" t="s">
+        <v>198</v>
+      </c>
       <c r="E7">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="F7">
-        <v>10</v>
+        <v>20</v>
+      </c>
+      <c r="G7">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>9</v>
+      </c>
+      <c r="I7" s="7">
+        <v>43011</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" s="19" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C8" s="20" t="s">
-        <v>183</v>
-      </c>
-      <c r="D8" s="20"/>
+        <v>176</v>
+      </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
       <c r="E8">
-        <v>20</v>
+        <v>65</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>15</v>
+      </c>
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>15</v>
+      </c>
+      <c r="I8" s="7">
+        <v>43011</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="B9" s="19" t="s">
-        <v>77</v>
+        <v>157</v>
       </c>
       <c r="C9" s="20" t="s">
-        <v>182</v>
-      </c>
-      <c r="D9" s="20"/>
+        <v>179</v>
+      </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
         <v>20</v>
       </c>
+      <c r="G9">
+        <v>12</v>
+      </c>
+      <c r="H9">
+        <v>12</v>
+      </c>
+      <c r="I9" s="7">
+        <v>43011</v>
+      </c>
     </row>
     <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A10" s="19" t="s">
-        <v>125</v>
-      </c>
-      <c r="B10" s="19" t="s">
-        <v>78</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>181</v>
-      </c>
-      <c r="E10">
-        <v>65</v>
-      </c>
-      <c r="F10">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="19" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="19" t="s">
-        <v>162</v>
-      </c>
-      <c r="C11" s="20" t="s">
-        <v>184</v>
-      </c>
-      <c r="D11" s="20"/>
-      <c r="E11">
-        <v>20</v>
-      </c>
-      <c r="F11">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="20"/>
+      <c r="B10" s="19"/>
+      <c r="C10" s="19"/>
+      <c r="D10" s="20"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="22"/>
+      <c r="I13" s="7"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B14" s="5" t="s">
+      <c r="B14" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="17" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>203</v>
+      </c>
+      <c r="I17" s="7"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B18" s="21"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B15" s="5"/>
-      <c r="I15" s="7"/>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="B16" s="5" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B17" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="18" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B18" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
-      <c r="B20" s="5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="B21" s="1" t="s">
-        <v>38</v>
-      </c>
+    <row r="20" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="21" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B22" s="21"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B23" s="21"/>
+    </row>
+    <row r="24" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B25" s="21"/>
+    </row>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="21"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B27" s="21"/>
+    </row>
+    <row r="28" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B28" s="21"/>
+    </row>
+    <row r="29" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B29" s="21"/>
+    </row>
+    <row r="30" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B30" s="21"/>
+    </row>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B31" s="21"/>
+    </row>
+    <row r="32" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B32" s="21"/>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B33" s="21"/>
+    </row>
+    <row r="34" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B34" s="21"/>
+    </row>
+    <row r="35" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B35" s="21"/>
+    </row>
+    <row r="36" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B36" s="21"/>
+    </row>
+    <row r="37" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B37" s="21"/>
+    </row>
+    <row r="38" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B38" s="21"/>
+    </row>
+    <row r="39" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B39" s="21"/>
+    </row>
+    <row r="40" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B40" s="21"/>
+    </row>
+    <row r="41" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B41" s="21"/>
+    </row>
+    <row r="42" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B42" s="21"/>
+    </row>
+    <row r="43" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B43" s="21"/>
+    </row>
+    <row r="44" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B44" s="21"/>
+    </row>
+    <row r="45" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B45" s="21"/>
+    </row>
+    <row r="46" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B46" s="21"/>
+    </row>
+    <row r="47" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B47" s="21"/>
+    </row>
+    <row r="48" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B48" s="21"/>
+    </row>
+    <row r="49" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B49" s="21"/>
+    </row>
+    <row r="50" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B50" s="21"/>
+    </row>
+    <row r="51" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B51" s="21"/>
+    </row>
+    <row r="52" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B52" s="21"/>
+    </row>
+    <row r="53" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B53" s="21"/>
+    </row>
+    <row r="54" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B54" s="21"/>
+    </row>
+    <row r="55" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B55" s="21"/>
+    </row>
+    <row r="56" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B56" s="21"/>
+    </row>
+    <row r="57" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B57" s="21"/>
+    </row>
+    <row r="58" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B58" s="21"/>
+    </row>
+    <row r="59" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B59" s="21"/>
+    </row>
+    <row r="60" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B60" s="21"/>
+    </row>
+    <row r="61" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B61" s="21"/>
+    </row>
+    <row r="62" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B62" s="21"/>
+    </row>
+    <row r="63" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B63" s="21"/>
+    </row>
+    <row r="64" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B64" s="21"/>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B65" s="21"/>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B66" s="21"/>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B67" s="21"/>
+    </row>
+    <row r="68" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B68" s="21"/>
+    </row>
+    <row r="69" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B69" s="21"/>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B70" s="21"/>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B71" s="21"/>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B72" s="21"/>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B73" s="21"/>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B74" s="21"/>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B75" s="21"/>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B76" s="21"/>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B77" s="21"/>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B78" s="21"/>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B79" s="21"/>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B80" s="21"/>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B81" s="21"/>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B82" s="21"/>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B83" s="21"/>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B84" s="21"/>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B85" s="21"/>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B86" s="21"/>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B87" s="21"/>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B88" s="21"/>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B89" s="21"/>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B90" s="21"/>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B91" s="21"/>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B92" s="21"/>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B93" s="21"/>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B94" s="21"/>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B95" s="21"/>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B96" s="21"/>
+    </row>
+    <row r="97" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B97" s="21"/>
+    </row>
+    <row r="98" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B98" s="21"/>
+    </row>
+    <row r="99" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B99" s="21"/>
+    </row>
+    <row r="100" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B100" s="21"/>
+    </row>
+    <row r="101" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B101" s="21"/>
+    </row>
+    <row r="102" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B102" s="21"/>
+    </row>
+    <row r="103" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B103" s="21"/>
+    </row>
+    <row r="104" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B104" s="21"/>
+    </row>
+    <row r="105" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B105" s="21"/>
+    </row>
+    <row r="106" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B106" s="21"/>
+    </row>
+    <row r="107" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B107" s="21"/>
+    </row>
+    <row r="108" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B108" s="21"/>
+    </row>
+    <row r="109" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B109" s="21"/>
+    </row>
+    <row r="110" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B110" s="21"/>
+    </row>
+    <row r="111" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B111" s="21"/>
+    </row>
+    <row r="112" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B112" s="21"/>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B113" s="21"/>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B114" s="21"/>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B115" s="21"/>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B116" s="21"/>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B117" s="21"/>
+    </row>
+    <row r="118" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B118" s="21"/>
+    </row>
+    <row r="119" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B119" s="21"/>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B120" s="21"/>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B121" s="21"/>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B122" s="21"/>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B123" s="21"/>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B124" s="21"/>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B125" s="21"/>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B126" s="21"/>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B127" s="21"/>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B128" s="21"/>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B129" s="21"/>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B130" s="21"/>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B131" s="21"/>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B132" s="21"/>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B133" s="21"/>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B134" s="21"/>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B135" s="21"/>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B136" s="21"/>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B137" s="21"/>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B138" s="21"/>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B139" s="21"/>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B140" s="21"/>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B141" s="21"/>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B142" s="21"/>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B143" s="21"/>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B144" s="21"/>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B145" s="21"/>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B146" s="21"/>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B147" s="21"/>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B148" s="21"/>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B149" s="21"/>
+    </row>
+    <row r="150" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B150" s="21"/>
+    </row>
+    <row r="151" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B151" s="21"/>
+    </row>
+    <row r="152" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B152" s="21"/>
+    </row>
+    <row r="153" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B153" s="21"/>
+    </row>
+    <row r="154" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B154" s="21"/>
+    </row>
+    <row r="155" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B155" s="21"/>
+    </row>
+    <row r="156" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B156" s="21"/>
+    </row>
+    <row r="157" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B157" s="21"/>
+    </row>
+    <row r="158" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B158" s="21"/>
+    </row>
+    <row r="159" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B159" s="21"/>
+    </row>
+    <row r="160" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B160" s="21"/>
+    </row>
+    <row r="161" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B161" s="21"/>
+    </row>
+    <row r="162" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B162" s="21"/>
+    </row>
+    <row r="163" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B163" s="21"/>
+    </row>
+    <row r="164" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B164" s="21"/>
+    </row>
+    <row r="165" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B165" s="21"/>
+    </row>
+    <row r="166" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B166" s="21"/>
+    </row>
+    <row r="167" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B167" s="21"/>
+    </row>
+    <row r="168" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B168" s="21"/>
+    </row>
+    <row r="169" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B169" s="21"/>
+    </row>
+    <row r="170" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B170" s="21"/>
+    </row>
+    <row r="171" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B171" s="21"/>
+    </row>
+    <row r="172" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B172" s="21"/>
+    </row>
+    <row r="173" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B173" s="21"/>
+    </row>
+    <row r="174" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B174" s="21"/>
+    </row>
+    <row r="175" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B175" s="21"/>
+    </row>
+    <row r="176" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B176" s="21"/>
+    </row>
+    <row r="177" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B177" s="21"/>
+    </row>
+    <row r="178" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B178" s="21"/>
+    </row>
+    <row r="179" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B179" s="21"/>
+    </row>
+    <row r="180" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B180" s="21"/>
+    </row>
+    <row r="181" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B181" s="21"/>
+    </row>
+    <row r="182" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B182" s="21"/>
+    </row>
+    <row r="183" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B183" s="21"/>
+    </row>
+    <row r="184" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B184" s="21"/>
+    </row>
+    <row r="185" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B185" s="21"/>
+    </row>
+    <row r="186" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B186" s="21"/>
+    </row>
+    <row r="187" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B187" s="21"/>
+    </row>
+    <row r="188" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B188" s="21"/>
+    </row>
+    <row r="189" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B189" s="21"/>
+    </row>
+    <row r="190" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B190" s="21"/>
+    </row>
+    <row r="191" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B191" s="21"/>
+    </row>
+    <row r="192" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B192" s="21"/>
+    </row>
+    <row r="193" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B193" s="21"/>
+    </row>
+    <row r="194" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B194" s="21"/>
+    </row>
+    <row r="195" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B195" s="21"/>
+    </row>
+    <row r="196" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B196" s="21"/>
+    </row>
+    <row r="197" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B197" s="21"/>
+    </row>
+    <row r="198" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B198" s="21"/>
+    </row>
+    <row r="199" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B199" s="21"/>
+    </row>
+    <row r="200" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B200" s="21"/>
+    </row>
+    <row r="201" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B201" s="21"/>
+    </row>
+    <row r="202" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B202" s="21"/>
+    </row>
+    <row r="203" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B203" s="21"/>
+    </row>
+    <row r="204" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B204" s="21"/>
+    </row>
+    <row r="205" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B205" s="21"/>
+    </row>
+    <row r="206" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B206" s="21"/>
+    </row>
+    <row r="207" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B207" s="21"/>
+    </row>
+    <row r="208" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B208" s="21"/>
+    </row>
+    <row r="209" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B209" s="21"/>
+    </row>
+    <row r="210" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B210" s="21"/>
+    </row>
+    <row r="211" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B211" s="21"/>
+    </row>
+    <row r="212" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B212" s="21"/>
+    </row>
+    <row r="213" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B213" s="21"/>
+    </row>
+    <row r="214" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B214" s="21"/>
+    </row>
+    <row r="215" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B215" s="21"/>
+    </row>
+    <row r="216" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B216" s="21"/>
+    </row>
+    <row r="217" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B217" s="21"/>
+    </row>
+    <row r="218" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B218" s="21"/>
+    </row>
+    <row r="219" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B219" s="21"/>
+    </row>
+    <row r="220" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B220" s="21"/>
+    </row>
+    <row r="221" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B221" s="21"/>
+    </row>
+    <row r="222" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B222" s="21"/>
+    </row>
+    <row r="223" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B223" s="21"/>
+    </row>
+    <row r="224" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B224" s="21"/>
+    </row>
+    <row r="225" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B225" s="21"/>
+    </row>
+    <row r="226" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B226" s="21"/>
+    </row>
+    <row r="227" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B227" s="21"/>
+    </row>
+    <row r="228" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B228" s="21"/>
+    </row>
+    <row r="229" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B229" s="21"/>
+    </row>
+    <row r="230" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B230" s="21"/>
+    </row>
+    <row r="231" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B231" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -3190,13 +3924,16 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -3225,6 +3962,142 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="19" t="s">
+        <v>122</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2">
+        <v>15</v>
+      </c>
+      <c r="F2">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" s="19" t="s">
+        <v>123</v>
+      </c>
+      <c r="B3" s="19" t="s">
+        <v>77</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" s="19" t="s">
+        <v>124</v>
+      </c>
+      <c r="B4" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" s="19" t="s">
+        <v>125</v>
+      </c>
+      <c r="B5" s="19" t="s">
+        <v>79</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5">
+        <v>15</v>
+      </c>
+      <c r="F5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" s="19" t="s">
+        <v>126</v>
+      </c>
+      <c r="B6" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6">
+        <v>35</v>
+      </c>
+      <c r="F6">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>127</v>
+      </c>
+      <c r="B7" s="19" t="s">
+        <v>170</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7">
+        <v>30</v>
+      </c>
+      <c r="F7">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" s="19" t="s">
+        <v>128</v>
+      </c>
+      <c r="B8" s="19" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8">
+        <v>35</v>
+      </c>
+      <c r="F8">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" s="19" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="19" t="s">
+        <v>83</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9">
+        <v>30</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -3328,8 +4201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3340,222 +4213,222 @@
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="B2" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>40</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>41</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="B4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="B5" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>71</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="B7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="B8" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>126</v>
+        <v>121</v>
       </c>
       <c r="B9" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="C9" s="12" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C10" s="12" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>128</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="C11" s="12" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>129</v>
+        <v>124</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C12" s="12" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>130</v>
+        <v>125</v>
       </c>
       <c r="B13" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="C13" s="12" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>131</v>
+        <v>126</v>
       </c>
       <c r="B14" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="C14" s="12" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B15" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B16" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B17" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C18" s="12" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
       <c r="B19" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="C19" s="12" t="s">
-        <v>51</v>
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C20" s="12" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="D20">
         <v>3</v>
@@ -3563,13 +4436,13 @@
     </row>
     <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="C21" s="12" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="D21">
         <v>3</v>
@@ -3577,170 +4450,170 @@
     </row>
     <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C22" s="12" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B23" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="C23" s="12" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="B24" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="B25" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="C25" s="12" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="B26" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="B27" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="C27" s="12" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="D27" t="s">
-        <v>202</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="B28" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="C28" s="12" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="B29" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="C29" s="12" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C30" s="12" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="C31" s="12" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="B32" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="C32" s="12" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="B33" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="C33" s="12" t="s">
-        <v>61</v>
+        <v>56</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="B34" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C34" s="12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
       <c r="B35" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="C35" s="12" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
       <c r="B36" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="C36" s="12" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D36">
         <v>2</v>
@@ -3748,13 +4621,13 @@
     </row>
     <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
       <c r="B37" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="C37" s="12" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="D37">
         <v>2</v>
@@ -3762,13 +4635,13 @@
     </row>
     <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B38" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D38">
         <v>2</v>
@@ -3776,13 +4649,13 @@
     </row>
     <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B39" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="C39" s="12" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D39">
         <v>2</v>
@@ -3790,13 +4663,13 @@
     </row>
     <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B40" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="C40" s="12" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D40">
         <v>2</v>
@@ -3804,24 +4677,24 @@
     </row>
     <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B41" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="C41" s="12" t="s">
-        <v>114</v>
+        <v>109</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B42" t="s">
-        <v>115</v>
+        <v>110</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="D42">
         <v>1</v>
@@ -3829,13 +4702,13 @@
     </row>
     <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
       <c r="C43" s="18" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="D43">
         <v>1</v>

</xml_diff>

<commit_message>
finish US11 and US15
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS-555-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1CEC31E-4517-49CF-B796-6C7B10A92F0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C8B926-008F-435B-9589-01B99F295292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3975" yWindow="1170" windowWidth="15825" windowHeight="10965" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="729" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
     <sheet name="Sprint4" sheetId="6" r:id="rId8"/>
     <sheet name="Stories" sheetId="11" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="181029" concurrentCalc="0"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -31,7 +31,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
@@ -43,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="390" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -1121,6 +1123,9 @@
                 <c:pt idx="1">
                   <c:v>43025</c:v>
                 </c:pt>
+                <c:pt idx="2">
+                  <c:v>43045</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1135,6 +1140,9 @@
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>24</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>16</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2028,12 +2036,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.5" customWidth="1"/>
-    <col min="3" max="3" width="8.5" customWidth="1"/>
-    <col min="4" max="5" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" customWidth="1"/>
+    <col min="3" max="3" width="8.453125" customWidth="1"/>
+    <col min="4" max="5" width="20.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2147,16 +2155,16 @@
   <dimension ref="A1:E33"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D17"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.125" customWidth="1"/>
-    <col min="2" max="2" width="7.625" customWidth="1"/>
-    <col min="3" max="3" width="23.5" customWidth="1"/>
-    <col min="4" max="4" width="6.625" customWidth="1"/>
-    <col min="5" max="5" width="7.625" customWidth="1"/>
+    <col min="1" max="1" width="5.08984375" customWidth="1"/>
+    <col min="2" max="2" width="7.6328125" customWidth="1"/>
+    <col min="3" max="3" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2176,7 +2184,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2193,7 +2201,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2210,7 +2218,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2227,7 +2235,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2244,7 +2252,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2261,7 +2269,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2278,7 +2286,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2295,7 +2303,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2312,7 +2320,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2327,7 +2335,7 @@
       </c>
       <c r="E10" s="19"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2342,7 +2350,7 @@
       </c>
       <c r="E11" s="19"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2355,9 +2363,11 @@
       <c r="D12" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E12" s="19"/>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E12" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2372,7 +2382,7 @@
       </c>
       <c r="E13" s="19"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2387,7 +2397,7 @@
       </c>
       <c r="E14" s="19"/>
     </row>
-    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2402,7 +2412,7 @@
       </c>
       <c r="E15" s="19"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2415,9 +2425,11 @@
       <c r="D16" s="20" t="s">
         <v>178</v>
       </c>
-      <c r="E16" s="19"/>
-    </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="E16" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2432,7 +2444,7 @@
       </c>
       <c r="E17" s="19"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2447,7 +2459,7 @@
       </c>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2462,7 +2474,7 @@
       </c>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2477,7 +2489,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2492,7 +2504,7 @@
       </c>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2507,7 +2519,7 @@
       </c>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2522,7 +2534,7 @@
       </c>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2537,7 +2549,7 @@
       </c>
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2552,7 +2564,7 @@
       </c>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2567,7 +2579,7 @@
       </c>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2582,7 +2594,7 @@
       </c>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2597,7 +2609,7 @@
       </c>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2612,7 +2624,7 @@
       </c>
       <c r="E29" s="19"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2627,7 +2639,7 @@
       </c>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2642,7 +2654,7 @@
       </c>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2657,7 +2669,7 @@
       </c>
       <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2683,18 +2695,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="7"/>
-    <col min="2" max="2" width="11.25" customWidth="1"/>
-    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.375" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="7"/>
+    <col min="2" max="2" width="11.26953125" customWidth="1"/>
+    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.36328125" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2875,20 +2887,20 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="7.125" customWidth="1"/>
-    <col min="5" max="5" width="6.875" customWidth="1"/>
-    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" style="2"/>
+    <col min="2" max="2" width="16.6328125" customWidth="1"/>
+    <col min="3" max="3" width="12.453125" customWidth="1"/>
+    <col min="4" max="4" width="7.08984375" customWidth="1"/>
+    <col min="5" max="5" width="6.90625" customWidth="1"/>
+    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2944,6 +2956,17 @@
       <c r="F3" s="9">
         <f>(D3-D2)/E3*60</f>
         <v>55.24752475247525</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="2">
+        <v>43045</v>
+      </c>
+      <c r="B4">
+        <v>16</v>
+      </c>
+      <c r="C4">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -2962,13 +2985,13 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.25" customWidth="1"/>
-    <col min="2" max="2" width="29.25" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.625" customWidth="1"/>
-    <col min="5" max="8" width="9.125" customWidth="1"/>
-    <col min="9" max="9" width="10.875" style="6"/>
+    <col min="1" max="1" width="9.26953125" customWidth="1"/>
+    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.6328125" customWidth="1"/>
+    <col min="5" max="8" width="9.08984375" customWidth="1"/>
+    <col min="9" max="9" width="10.90625" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3000,7 +3023,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>114</v>
       </c>
@@ -3029,7 +3052,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>115</v>
       </c>
@@ -3058,7 +3081,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>116</v>
       </c>
@@ -3087,7 +3110,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>117</v>
       </c>
@@ -3116,7 +3139,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>118</v>
       </c>
@@ -3145,7 +3168,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>119</v>
       </c>
@@ -3174,7 +3197,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>120</v>
       </c>
@@ -3203,7 +3226,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>121</v>
       </c>
@@ -3232,7 +3255,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
@@ -3926,16 +3949,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -3964,7 +3987,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -3981,7 +4004,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>123</v>
       </c>
@@ -3998,7 +4021,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>124</v>
       </c>
@@ -4015,7 +4038,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>125</v>
       </c>
@@ -4032,7 +4055,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>126</v>
       </c>
@@ -4049,7 +4072,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>127</v>
       </c>
@@ -4066,7 +4089,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>128</v>
       </c>
@@ -4083,7 +4106,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>129</v>
       </c>
@@ -4115,9 +4138,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4160,9 +4183,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4201,14 +4224,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4222,7 +4245,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4233,7 +4256,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4244,7 +4267,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4255,7 +4278,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4266,7 +4289,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4277,7 +4300,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4288,7 +4311,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4299,7 +4322,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4310,7 +4333,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4321,7 +4344,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4332,7 +4355,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4343,7 +4366,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4354,7 +4377,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4365,7 +4388,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4376,7 +4399,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4387,7 +4410,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4398,7 +4421,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4409,7 +4432,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4420,7 +4443,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4434,7 +4457,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4448,7 +4471,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4459,7 +4482,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4470,7 +4493,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4481,7 +4504,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4492,7 +4515,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4503,7 +4526,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="126" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4517,7 +4540,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4528,7 +4551,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4539,7 +4562,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4550,7 +4573,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4561,7 +4584,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4572,7 +4595,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4583,7 +4606,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4594,7 +4617,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4605,7 +4628,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4619,7 +4642,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4633,7 +4656,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4647,7 +4670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4661,7 +4684,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4675,7 +4698,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4686,7 +4709,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4700,7 +4723,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Sprint 2 retrospective and sprint 3 planning report
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -5,12 +5,12 @@
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CS-555-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C8B926-008F-435B-9589-01B99F295292}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052973F7-9AE8-475A-BF9A-7FF96B87F363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" tabRatio="729" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1500" yWindow="2775" windowWidth="31665" windowHeight="11535" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="204">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="211">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -687,6 +687,27 @@
   </si>
   <si>
     <t>Helping eachother with dev environment setup</t>
+  </si>
+  <si>
+    <t>Writing our own test cases</t>
+  </si>
+  <si>
+    <t>Testing our code</t>
+  </si>
+  <si>
+    <t>Taking design inspiration from previous user stories and user stories from this sprint from other people</t>
+  </si>
+  <si>
+    <t>Adding unneeded import</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Leaning heavily on SQL </t>
+  </si>
+  <si>
+    <t>Not testing the code</t>
+  </si>
+  <si>
+    <t>Not writing user stories</t>
   </si>
 </sst>
 </file>
@@ -2036,12 +2057,12 @@
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="7.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.453125" customWidth="1"/>
-    <col min="3" max="3" width="8.453125" customWidth="1"/>
-    <col min="4" max="5" width="20.453125" customWidth="1"/>
+    <col min="1" max="1" width="7.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.5" customWidth="1"/>
+    <col min="3" max="3" width="8.5" customWidth="1"/>
+    <col min="4" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2154,17 +2175,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.08984375" customWidth="1"/>
-    <col min="2" max="2" width="7.6328125" customWidth="1"/>
-    <col min="3" max="3" width="23.453125" customWidth="1"/>
-    <col min="4" max="4" width="6.6328125" customWidth="1"/>
-    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="1" max="1" width="5.125" customWidth="1"/>
+    <col min="2" max="2" width="7.625" customWidth="1"/>
+    <col min="3" max="3" width="23.5" customWidth="1"/>
+    <col min="4" max="4" width="6.625" customWidth="1"/>
+    <col min="5" max="5" width="7.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2184,7 +2205,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2201,7 +2222,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -2218,7 +2239,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -2235,7 +2256,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -2252,7 +2273,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -2269,7 +2290,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -2286,7 +2307,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -2303,7 +2324,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2320,7 +2341,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>2</v>
       </c>
@@ -2333,9 +2354,11 @@
       <c r="D10" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="E10" s="19"/>
-    </row>
-    <row r="11" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E10" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>2</v>
       </c>
@@ -2348,9 +2371,11 @@
       <c r="D11" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="E11" s="19"/>
-    </row>
-    <row r="12" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E11" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>2</v>
       </c>
@@ -2367,7 +2392,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>2</v>
       </c>
@@ -2380,9 +2405,11 @@
       <c r="D13" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="19"/>
-    </row>
-    <row r="14" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E13" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>2</v>
       </c>
@@ -2395,9 +2422,11 @@
       <c r="D14" s="20" t="s">
         <v>176</v>
       </c>
-      <c r="E14" s="19"/>
-    </row>
-    <row r="15" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E14" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -2410,9 +2439,11 @@
       <c r="D15" s="20" t="s">
         <v>177</v>
       </c>
-      <c r="E15" s="19"/>
-    </row>
-    <row r="16" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E15" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>2</v>
       </c>
@@ -2429,7 +2460,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="17" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>2</v>
       </c>
@@ -2442,9 +2473,11 @@
       <c r="D17" s="20" t="s">
         <v>179</v>
       </c>
-      <c r="E17" s="19"/>
-    </row>
-    <row r="18" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+      <c r="E17" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2459,7 +2492,7 @@
       </c>
       <c r="E18" s="19"/>
     </row>
-    <row r="19" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2474,7 +2507,7 @@
       </c>
       <c r="E19" s="19"/>
     </row>
-    <row r="20" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2489,7 +2522,7 @@
       </c>
       <c r="E20" s="19"/>
     </row>
-    <row r="21" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2504,7 +2537,7 @@
       </c>
       <c r="E21" s="19"/>
     </row>
-    <row r="22" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
@@ -2519,7 +2552,7 @@
       </c>
       <c r="E22" s="19"/>
     </row>
-    <row r="23" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
@@ -2534,7 +2567,7 @@
       </c>
       <c r="E23" s="19"/>
     </row>
-    <row r="24" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
@@ -2549,7 +2582,7 @@
       </c>
       <c r="E24" s="19"/>
     </row>
-    <row r="25" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
@@ -2564,7 +2597,7 @@
       </c>
       <c r="E25" s="19"/>
     </row>
-    <row r="26" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2579,7 +2612,7 @@
       </c>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
@@ -2594,7 +2627,7 @@
       </c>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
@@ -2609,7 +2642,7 @@
       </c>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
@@ -2624,7 +2657,7 @@
       </c>
       <c r="E29" s="19"/>
     </row>
-    <row r="30" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
@@ -2639,7 +2672,7 @@
       </c>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
@@ -2654,7 +2687,7 @@
       </c>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
@@ -2669,7 +2702,7 @@
       </c>
       <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="1:5" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
@@ -2695,18 +2728,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="7"/>
-    <col min="2" max="2" width="11.26953125" customWidth="1"/>
-    <col min="3" max="3" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.36328125" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="7"/>
+    <col min="2" max="2" width="11.25" customWidth="1"/>
+    <col min="3" max="3" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.375" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
@@ -2893,14 +2926,14 @@
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.90625" style="2"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="3" width="12.453125" customWidth="1"/>
-    <col min="4" max="4" width="7.08984375" customWidth="1"/>
-    <col min="5" max="5" width="6.90625" customWidth="1"/>
-    <col min="6" max="6" width="12.453125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="10.875" style="2"/>
+    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="7.125" customWidth="1"/>
+    <col min="5" max="5" width="6.875" customWidth="1"/>
+    <col min="6" max="6" width="12.5" style="9" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -2981,17 +3014,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11:B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.26953125" customWidth="1"/>
-    <col min="2" max="2" width="29.26953125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="6.6328125" customWidth="1"/>
-    <col min="5" max="8" width="9.08984375" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="6"/>
+    <col min="1" max="1" width="9.25" customWidth="1"/>
+    <col min="2" max="2" width="29.25" style="1" customWidth="1"/>
+    <col min="3" max="3" width="6.625" customWidth="1"/>
+    <col min="5" max="8" width="9.125" customWidth="1"/>
+    <col min="9" max="9" width="10.875" style="6"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -3023,7 +3056,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>114</v>
       </c>
@@ -3052,7 +3085,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>115</v>
       </c>
@@ -3081,7 +3114,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>116</v>
       </c>
@@ -3110,7 +3143,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>117</v>
       </c>
@@ -3139,7 +3172,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>118</v>
       </c>
@@ -3168,7 +3201,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>119</v>
       </c>
@@ -3197,7 +3230,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>120</v>
       </c>
@@ -3226,7 +3259,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>121</v>
       </c>
@@ -3255,7 +3288,7 @@
         <v>43011</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B10" s="19"/>
       <c r="C10" s="19"/>
       <c r="D10" s="20"/>
@@ -3947,13 +3980,13 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="25" customWidth="1"/>
   </cols>
@@ -3987,7 +4020,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A2" s="19" t="s">
         <v>122</v>
       </c>
@@ -3997,14 +4030,26 @@
       <c r="C2" s="20" t="s">
         <v>176</v>
       </c>
+      <c r="D2" t="s">
+        <v>198</v>
+      </c>
       <c r="E2">
         <v>15</v>
       </c>
       <c r="F2">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G2">
+        <v>17</v>
+      </c>
+      <c r="H2">
+        <v>7</v>
+      </c>
+      <c r="I2" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" s="19" t="s">
         <v>123</v>
       </c>
@@ -4014,14 +4059,26 @@
       <c r="C3" s="20" t="s">
         <v>177</v>
       </c>
+      <c r="D3" t="s">
+        <v>198</v>
+      </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
         <v>15</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G3">
+        <v>26</v>
+      </c>
+      <c r="H3">
+        <v>40</v>
+      </c>
+      <c r="I3" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" s="19" t="s">
         <v>124</v>
       </c>
@@ -4031,14 +4088,27 @@
       <c r="C4" s="20" t="s">
         <v>178</v>
       </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
       <c r="E4">
         <v>20</v>
       </c>
       <c r="F4">
         <v>15</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G4">
+        <f>269-231</f>
+        <v>38</v>
+      </c>
+      <c r="H4">
+        <v>35</v>
+      </c>
+      <c r="I4" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A5" s="19" t="s">
         <v>125</v>
       </c>
@@ -4048,14 +4118,27 @@
       <c r="C5" s="20" t="s">
         <v>179</v>
       </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
       <c r="E5">
         <v>15</v>
       </c>
       <c r="F5">
         <v>10</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G5">
+        <f>91-75</f>
+        <v>16</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A6" s="19" t="s">
         <v>126</v>
       </c>
@@ -4065,14 +4148,27 @@
       <c r="C6" s="20" t="s">
         <v>176</v>
       </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
       <c r="E6">
         <v>35</v>
       </c>
       <c r="F6">
         <v>25</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G6">
+        <f>119-98</f>
+        <v>21</v>
+      </c>
+      <c r="H6">
+        <v>12</v>
+      </c>
+      <c r="I6" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A7" s="19" t="s">
         <v>127</v>
       </c>
@@ -4082,14 +4178,27 @@
       <c r="C7" s="20" t="s">
         <v>177</v>
       </c>
+      <c r="D7" t="s">
+        <v>198</v>
+      </c>
       <c r="E7">
         <v>30</v>
       </c>
       <c r="F7">
         <v>25</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G7">
+        <f>51-24</f>
+        <v>27</v>
+      </c>
+      <c r="H7">
+        <v>23</v>
+      </c>
+      <c r="I7" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A8" s="19" t="s">
         <v>128</v>
       </c>
@@ -4099,14 +4208,26 @@
       <c r="C8" s="20" t="s">
         <v>178</v>
       </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
       <c r="E8">
         <v>35</v>
       </c>
       <c r="F8">
         <v>25</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G8">
+        <v>10</v>
+      </c>
+      <c r="H8">
+        <v>45</v>
+      </c>
+      <c r="I8" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A9" s="19" t="s">
         <v>129</v>
       </c>
@@ -4116,12 +4237,86 @@
       <c r="C9" s="20" t="s">
         <v>179</v>
       </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
       <c r="E9">
         <v>30</v>
       </c>
       <c r="F9">
         <v>20</v>
       </c>
+      <c r="G9">
+        <v>14</v>
+      </c>
+      <c r="H9">
+        <v>20</v>
+      </c>
+      <c r="I9" s="13">
+        <v>43046</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="22"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="21"/>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4132,13 +4327,16 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="27.75" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
@@ -4167,6 +4365,142 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>130</v>
+      </c>
+      <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2">
+        <v>30</v>
+      </c>
+      <c r="F2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B3" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>132</v>
+      </c>
+      <c r="B4" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4">
+        <v>40</v>
+      </c>
+      <c r="F4">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>133</v>
+      </c>
+      <c r="B5" t="s">
+        <v>87</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>134</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
+      <c r="C6" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6">
+        <v>8</v>
+      </c>
+      <c r="F6">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>135</v>
+      </c>
+      <c r="B7" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="20" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7">
+        <v>8</v>
+      </c>
+      <c r="F7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>136</v>
+      </c>
+      <c r="B8" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="20" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8">
+        <v>8</v>
+      </c>
+      <c r="F8">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B9" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="20" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>25</v>
       </c>
     </row>
   </sheetData>
@@ -4183,9 +4517,9 @@
       <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4224,14 +4558,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="F24" sqref="F24"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18:B25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.6" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="28.08984375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="49.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="28.125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="49.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="4" customFormat="1" x14ac:dyDescent="0.2">
@@ -4245,7 +4579,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>114</v>
       </c>
@@ -4256,7 +4590,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>115</v>
       </c>
@@ -4267,7 +4601,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>116</v>
       </c>
@@ -4278,7 +4612,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>117</v>
       </c>
@@ -4289,7 +4623,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>118</v>
       </c>
@@ -4300,7 +4634,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>119</v>
       </c>
@@ -4311,7 +4645,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>120</v>
       </c>
@@ -4322,7 +4656,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>121</v>
       </c>
@@ -4333,7 +4667,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>122</v>
       </c>
@@ -4344,7 +4678,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>123</v>
       </c>
@@ -4355,7 +4689,7 @@
         <v>172</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>124</v>
       </c>
@@ -4366,7 +4700,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>125</v>
       </c>
@@ -4377,7 +4711,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="45" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="63" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>126</v>
       </c>
@@ -4388,7 +4722,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>127</v>
       </c>
@@ -4399,7 +4733,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>128</v>
       </c>
@@ -4410,7 +4744,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>129</v>
       </c>
@@ -4421,7 +4755,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>130</v>
       </c>
@@ -4432,7 +4766,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -4443,7 +4777,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>132</v>
       </c>
@@ -4457,7 +4791,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>133</v>
       </c>
@@ -4471,7 +4805,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>134</v>
       </c>
@@ -4482,7 +4816,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>135</v>
       </c>
@@ -4493,7 +4827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>136</v>
       </c>
@@ -4504,7 +4838,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>137</v>
       </c>
@@ -4515,7 +4849,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>138</v>
       </c>
@@ -4526,7 +4860,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="105" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4" ht="126" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>139</v>
       </c>
@@ -4540,7 +4874,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>
@@ -4551,7 +4885,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>141</v>
       </c>
@@ -4562,7 +4896,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>142</v>
       </c>
@@ -4573,7 +4907,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>143</v>
       </c>
@@ -4584,7 +4918,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>144</v>
       </c>
@@ -4595,7 +4929,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>145</v>
       </c>
@@ -4606,7 +4940,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>146</v>
       </c>
@@ -4617,7 +4951,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:4" ht="47.25" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>147</v>
       </c>
@@ -4628,7 +4962,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>148</v>
       </c>
@@ -4642,7 +4976,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>149</v>
       </c>
@@ -4656,7 +4990,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>150</v>
       </c>
@@ -4670,7 +5004,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>151</v>
       </c>
@@ -4684,7 +5018,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>152</v>
       </c>
@@ -4698,7 +5032,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>153</v>
       </c>
@@ -4709,7 +5043,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>154</v>
       </c>
@@ -4723,7 +5057,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>155</v>
       </c>

</xml_diff>

<commit_message>
Sprint 3 finished, sprint 4 started
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{052973F7-9AE8-475A-BF9A-7FF96B87F363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EF88B9-9AC0-4BF7-83E3-84096DE7A8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1500" yWindow="2775" windowWidth="31665" windowHeight="11535" tabRatio="729" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18585" yWindow="630" windowWidth="18450" windowHeight="12450" tabRatio="729" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="214">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -708,6 +708,15 @@
   </si>
   <si>
     <t>Not writing user stories</t>
+  </si>
+  <si>
+    <t>Writing our code in a vacuum: not looking at the other implementations.</t>
+  </si>
+  <si>
+    <t>Not taking inspiration from the other user stories.</t>
+  </si>
+  <si>
+    <t>Not providing feedback to the other user stories.</t>
   </si>
 </sst>
 </file>
@@ -1147,6 +1156,9 @@
                 <c:pt idx="2">
                   <c:v>43045</c:v>
                 </c:pt>
+                <c:pt idx="3">
+                  <c:v>43057</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1164,6 +1176,9 @@
                 </c:pt>
                 <c:pt idx="2">
                   <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2054,7 +2069,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2173,10 +2188,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:E33"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2471,7 +2486,7 @@
         <v>83</v>
       </c>
       <c r="D17" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E17" s="19" t="s">
         <v>198</v>
@@ -2488,9 +2503,11 @@
         <v>84</v>
       </c>
       <c r="D18" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E18" s="19"/>
+        <v>177</v>
+      </c>
+      <c r="E18" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A19">
@@ -2503,112 +2520,126 @@
         <v>85</v>
       </c>
       <c r="D19" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E19" s="19"/>
+        <v>178</v>
+      </c>
+      <c r="E19" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
       <c r="B20" s="19" t="s">
-        <v>134</v>
-      </c>
-      <c r="C20" s="19" t="s">
-        <v>88</v>
+        <v>132</v>
+      </c>
+      <c r="C20" t="s">
+        <v>86</v>
       </c>
       <c r="D20" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E20" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="21" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
       <c r="B21" s="19" t="s">
-        <v>135</v>
-      </c>
-      <c r="C21" s="19" t="s">
-        <v>91</v>
+        <v>133</v>
+      </c>
+      <c r="C21" t="s">
+        <v>87</v>
       </c>
       <c r="D21" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="E21" s="19"/>
+        <v>176</v>
+      </c>
+      <c r="E21" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>3</v>
       </c>
       <c r="B22" s="19" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C22" s="19" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="D22" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E22" s="19"/>
+        <v>177</v>
+      </c>
+      <c r="E22" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>3</v>
       </c>
       <c r="B23" s="19" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C23" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D23" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E23" s="19"/>
+        <v>178</v>
+      </c>
+      <c r="E23" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>3</v>
       </c>
       <c r="B24" s="19" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C24" s="19" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D24" s="20" t="s">
-        <v>178</v>
-      </c>
-      <c r="E24" s="19"/>
+        <v>179</v>
+      </c>
+      <c r="E24" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>3</v>
       </c>
       <c r="B25" s="19" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C25" s="19" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="D25" s="20" t="s">
-        <v>179</v>
-      </c>
-      <c r="E25" s="19"/>
+        <v>177</v>
+      </c>
+      <c r="E25" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
       <c r="B26" s="19" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C26" s="19" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D26" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E26" s="19"/>
     </row>
@@ -2617,13 +2648,13 @@
         <v>4</v>
       </c>
       <c r="B27" s="19" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="D27" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E27" s="19"/>
     </row>
@@ -2632,13 +2663,13 @@
         <v>4</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="D28" s="20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E28" s="19"/>
     </row>
@@ -2647,13 +2678,13 @@
         <v>4</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D29" s="20" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="E29" s="19"/>
     </row>
@@ -2662,13 +2693,13 @@
         <v>4</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="D30" s="20" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="E30" s="19"/>
     </row>
@@ -2677,13 +2708,13 @@
         <v>4</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="D31" s="20" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E31" s="19"/>
     </row>
@@ -2692,13 +2723,13 @@
         <v>4</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>112</v>
+        <v>101</v>
       </c>
       <c r="D32" s="20" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E32" s="19"/>
     </row>
@@ -2707,15 +2738,27 @@
         <v>4</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>108</v>
+        <v>102</v>
       </c>
       <c r="D33" s="20" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E33" s="19"/>
+    </row>
+    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B34" s="19"/>
+      <c r="C34" s="19"/>
+      <c r="D34" s="20"/>
+      <c r="E34" s="19"/>
+    </row>
+    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+      <c r="B35" s="19"/>
+      <c r="C35" s="19"/>
+      <c r="D35" s="20"/>
+      <c r="E35" s="19"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -2920,16 +2963,16 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.875" style="2"/>
-    <col min="2" max="2" width="16.625" customWidth="1"/>
+    <col min="2" max="2" width="22.125" customWidth="1"/>
     <col min="3" max="3" width="12.5" customWidth="1"/>
     <col min="4" max="4" width="7.125" customWidth="1"/>
     <col min="5" max="5" width="6.875" customWidth="1"/>
@@ -2999,7 +3042,44 @@
         <v>16</v>
       </c>
       <c r="C4">
+        <f t="shared" ref="C4:C5" si="0">B3-B4</f>
         <v>8</v>
+      </c>
+      <c r="D4">
+        <f>SUM(Sprint2!G:G)</f>
+        <v>169</v>
+      </c>
+      <c r="E4">
+        <f>SUM(Sprint2!H:H)</f>
+        <v>207</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" ref="F4:F5" si="1">(D4-D3)/E4*60</f>
+        <v>22.028985507246379</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="2">
+        <v>43057</v>
+      </c>
+      <c r="B5">
+        <v>8</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D5">
+        <f>SUM(Sprint3!G:G)</f>
+        <v>203</v>
+      </c>
+      <c r="E5">
+        <f>SUM(Sprint3!H:H)</f>
+        <v>202</v>
+      </c>
+      <c r="F5" s="9">
+        <f t="shared" si="1"/>
+        <v>10.099009900990099</v>
       </c>
     </row>
   </sheetData>
@@ -3982,9 +4062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:I25"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
-    </sheetView>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
@@ -4327,10 +4405,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="C2" sqref="C2:C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4377,11 +4455,23 @@
       <c r="C2" s="20" t="s">
         <v>176</v>
       </c>
+      <c r="D2" t="s">
+        <v>198</v>
+      </c>
       <c r="E2">
         <v>30</v>
       </c>
       <c r="F2">
         <v>35</v>
+      </c>
+      <c r="G2">
+        <v>19</v>
+      </c>
+      <c r="H2">
+        <v>60</v>
+      </c>
+      <c r="I2" s="13">
+        <v>43057</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4394,11 +4484,20 @@
       <c r="C3" s="20" t="s">
         <v>177</v>
       </c>
+      <c r="D3" t="s">
+        <v>198</v>
+      </c>
       <c r="E3">
         <v>20</v>
       </c>
       <c r="F3">
         <v>15</v>
+      </c>
+      <c r="G3">
+        <v>23</v>
+      </c>
+      <c r="H3">
+        <v>25</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4411,11 +4510,20 @@
       <c r="C4" s="20" t="s">
         <v>178</v>
       </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
       <c r="E4">
         <v>40</v>
       </c>
       <c r="F4">
         <v>45</v>
+      </c>
+      <c r="G4">
+        <v>45</v>
+      </c>
+      <c r="H4">
+        <v>28</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4428,11 +4536,20 @@
       <c r="C5" s="20" t="s">
         <v>179</v>
       </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
       <c r="E5">
         <v>20</v>
       </c>
       <c r="F5">
         <v>20</v>
+      </c>
+      <c r="G5">
+        <v>20</v>
+      </c>
+      <c r="H5">
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4445,11 +4562,20 @@
       <c r="C6" s="20" t="s">
         <v>176</v>
       </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
       <c r="E6">
         <v>8</v>
       </c>
       <c r="F6">
         <v>5</v>
+      </c>
+      <c r="G6">
+        <v>23</v>
+      </c>
+      <c r="H6">
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4462,11 +4588,20 @@
       <c r="C7" s="20" t="s">
         <v>177</v>
       </c>
+      <c r="D7" t="s">
+        <v>198</v>
+      </c>
       <c r="E7">
         <v>8</v>
       </c>
       <c r="F7">
         <v>5</v>
+      </c>
+      <c r="G7">
+        <v>35</v>
+      </c>
+      <c r="H7">
+        <v>30</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="15.75" x14ac:dyDescent="0.2">
@@ -4479,10 +4614,19 @@
       <c r="C8" s="20" t="s">
         <v>178</v>
       </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
       <c r="E8">
         <v>8</v>
       </c>
       <c r="F8">
+        <v>5</v>
+      </c>
+      <c r="G8">
+        <v>25</v>
+      </c>
+      <c r="H8">
         <v>5</v>
       </c>
     </row>
@@ -4496,12 +4640,83 @@
       <c r="C9" s="20" t="s">
         <v>179</v>
       </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
         <v>25</v>
       </c>
+      <c r="G9">
+        <v>13</v>
+      </c>
+      <c r="H9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="22"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="21" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="21" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="21" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B23" s="21" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B24" s="21" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B25" s="21"/>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B26" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -4511,15 +4726,18 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I1"/>
+  <dimension ref="A1:I9"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="24.875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="25.5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
@@ -4546,6 +4764,142 @@
       </c>
       <c r="I1" s="10" t="s">
         <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>138</v>
+      </c>
+      <c r="B2" t="s">
+        <v>94</v>
+      </c>
+      <c r="C2" t="s">
+        <v>176</v>
+      </c>
+      <c r="E2">
+        <v>25</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E3">
+        <v>10</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B4" t="s">
+        <v>96</v>
+      </c>
+      <c r="C4" t="s">
+        <v>178</v>
+      </c>
+      <c r="E4">
+        <v>45</v>
+      </c>
+      <c r="F4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>141</v>
+      </c>
+      <c r="B5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C5" t="s">
+        <v>179</v>
+      </c>
+      <c r="E5">
+        <v>25</v>
+      </c>
+      <c r="F5">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>142</v>
+      </c>
+      <c r="B6" t="s">
+        <v>98</v>
+      </c>
+      <c r="C6" t="s">
+        <v>176</v>
+      </c>
+      <c r="E6">
+        <v>15</v>
+      </c>
+      <c r="F6">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>143</v>
+      </c>
+      <c r="B7" t="s">
+        <v>99</v>
+      </c>
+      <c r="C7" t="s">
+        <v>177</v>
+      </c>
+      <c r="E7">
+        <v>50</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>144</v>
+      </c>
+      <c r="B8" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" t="s">
+        <v>178</v>
+      </c>
+      <c r="E8">
+        <v>10</v>
+      </c>
+      <c r="F8">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B9" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" t="s">
+        <v>179</v>
+      </c>
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -4558,8 +4912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:B25"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20:B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updates to the report after US 28 and 32 done
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63EF88B9-9AC0-4BF7-83E3-84096DE7A8A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4297A232-D983-437C-8168-423D35F27494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18585" yWindow="630" windowWidth="18450" windowHeight="12450" tabRatio="729" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19815" yWindow="525" windowWidth="18450" windowHeight="12450" tabRatio="729" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="214">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -2190,8 +2190,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2628,7 +2628,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>4</v>
       </c>
@@ -2638,115 +2638,119 @@
       <c r="C26" s="19" t="s">
         <v>94</v>
       </c>
-      <c r="D26" s="20" t="s">
-        <v>177</v>
+      <c r="D26" t="s">
+        <v>176</v>
       </c>
       <c r="E26" s="19"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>4</v>
       </c>
-      <c r="B27" s="19" t="s">
-        <v>140</v>
+      <c r="B27" t="s">
+        <v>139</v>
       </c>
       <c r="C27" s="19" t="s">
-        <v>96</v>
-      </c>
-      <c r="D27" s="20" t="s">
-        <v>178</v>
+        <v>95</v>
+      </c>
+      <c r="D27" t="s">
+        <v>177</v>
       </c>
       <c r="E27" s="19"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>4</v>
       </c>
       <c r="B28" s="19" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C28" s="19" t="s">
-        <v>97</v>
-      </c>
-      <c r="D28" s="20" t="s">
-        <v>179</v>
+        <v>96</v>
+      </c>
+      <c r="D28" t="s">
+        <v>178</v>
       </c>
       <c r="E28" s="19"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>4</v>
       </c>
       <c r="B29" s="19" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C29" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="D29" s="20" t="s">
-        <v>176</v>
-      </c>
-      <c r="E29" s="19"/>
-    </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+        <v>97</v>
+      </c>
+      <c r="D29" t="s">
+        <v>179</v>
+      </c>
+      <c r="E29" s="19" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>4</v>
       </c>
       <c r="B30" s="19" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C30" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="D30" s="20" t="s">
-        <v>177</v>
+        <v>98</v>
+      </c>
+      <c r="D30" t="s">
+        <v>176</v>
       </c>
       <c r="E30" s="19"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>4</v>
       </c>
       <c r="B31" s="19" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C31" s="19" t="s">
-        <v>100</v>
-      </c>
-      <c r="D31" s="20" t="s">
-        <v>178</v>
+        <v>99</v>
+      </c>
+      <c r="D31" t="s">
+        <v>177</v>
       </c>
       <c r="E31" s="19"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>4</v>
       </c>
       <c r="B32" s="19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C32" s="19" t="s">
-        <v>101</v>
-      </c>
-      <c r="D32" s="20" t="s">
-        <v>179</v>
+        <v>100</v>
+      </c>
+      <c r="D32" t="s">
+        <v>178</v>
       </c>
       <c r="E32" s="19"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>4</v>
       </c>
       <c r="B33" s="19" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C33" s="19" t="s">
-        <v>102</v>
-      </c>
-      <c r="D33" s="20" t="s">
-        <v>177</v>
-      </c>
-      <c r="E33" s="19"/>
+        <v>101</v>
+      </c>
+      <c r="D33" t="s">
+        <v>179</v>
+      </c>
+      <c r="E33" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B34" s="19"/>
@@ -4729,7 +4733,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4827,11 +4831,23 @@
       <c r="C5" t="s">
         <v>179</v>
       </c>
+      <c r="D5" t="s">
+        <v>198</v>
+      </c>
       <c r="E5">
         <v>25</v>
       </c>
       <c r="F5">
         <v>50</v>
+      </c>
+      <c r="G5">
+        <v>21</v>
+      </c>
+      <c r="H5">
+        <v>25</v>
+      </c>
+      <c r="I5" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -4895,11 +4911,23 @@
       <c r="C9" t="s">
         <v>179</v>
       </c>
+      <c r="D9" t="s">
+        <v>198</v>
+      </c>
       <c r="E9">
         <v>20</v>
       </c>
       <c r="F9">
         <v>10</v>
+      </c>
+      <c r="G9">
+        <v>20</v>
+      </c>
+      <c r="H9">
+        <v>35</v>
+      </c>
+      <c r="I9" s="13">
+        <v>43070</v>
       </c>
     </row>
   </sheetData>
@@ -4912,8 +4940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20:B21"/>
+    <sheetView topLeftCell="A25" zoomScale="85" zoomScaleNormal="85" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Updated report doc at end of sprint 4
</commit_message>
<xml_diff>
--- a/TeamAMNSReport.xlsx
+++ b/TeamAMNSReport.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\andrew\GEDCOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4297A232-D983-437C-8168-423D35F27494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE1EFC45-4CB6-4847-8C58-0EDB99E6BD41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19815" yWindow="525" windowWidth="18450" windowHeight="12450" tabRatio="729" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="14790" yWindow="1020" windowWidth="21975" windowHeight="11385" tabRatio="729" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Team" sheetId="1" r:id="rId1"/>
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="214">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="514" uniqueCount="219">
   <si>
     <t>Date</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -717,6 +717,21 @@
   </si>
   <si>
     <t>Not providing feedback to the other user stories.</t>
+  </si>
+  <si>
+    <t>Doing things in SQL when possible</t>
+  </si>
+  <si>
+    <t>Keeping implementations of similar things the same between user stories</t>
+  </si>
+  <si>
+    <t>Trying to make the output the same for all user stories</t>
+  </si>
+  <si>
+    <t>Writing code in a vacuum, without knowing what the other user stories are doing</t>
+  </si>
+  <si>
+    <t>Designing the architecture without all the user stories in mind</t>
   </si>
 </sst>
 </file>
@@ -1159,6 +1174,9 @@
                 <c:pt idx="3">
                   <c:v>43057</c:v>
                 </c:pt>
+                <c:pt idx="4">
+                  <c:v>43070</c:v>
+                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
@@ -1179,6 +1197,9 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2190,8 +2211,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E35"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C35" sqref="C35"/>
+    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2641,7 +2662,9 @@
       <c r="D26" t="s">
         <v>176</v>
       </c>
-      <c r="E26" s="19"/>
+      <c r="E26" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27">
@@ -2656,7 +2679,9 @@
       <c r="D27" t="s">
         <v>177</v>
       </c>
-      <c r="E27" s="19"/>
+      <c r="E27" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28">
@@ -2671,7 +2696,9 @@
       <c r="D28" t="s">
         <v>178</v>
       </c>
-      <c r="E28" s="19"/>
+      <c r="E28" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29">
@@ -2703,7 +2730,9 @@
       <c r="D30" t="s">
         <v>176</v>
       </c>
-      <c r="E30" s="19"/>
+      <c r="E30" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31">
@@ -2718,7 +2747,9 @@
       <c r="D31" t="s">
         <v>177</v>
       </c>
-      <c r="E31" s="19"/>
+      <c r="E31" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32">
@@ -2733,7 +2764,9 @@
       <c r="D32" t="s">
         <v>178</v>
       </c>
-      <c r="E32" s="19"/>
+      <c r="E32" s="19" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33">
@@ -2775,7 +2808,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:G19"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
@@ -2967,10 +3000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3046,7 +3079,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <f t="shared" ref="C4:C5" si="0">B3-B4</f>
+        <f t="shared" ref="C4:C6" si="0">B3-B4</f>
         <v>8</v>
       </c>
       <c r="D4">
@@ -3058,7 +3091,7 @@
         <v>207</v>
       </c>
       <c r="F4" s="9">
-        <f t="shared" ref="F4:F5" si="1">(D4-D3)/E4*60</f>
+        <f t="shared" ref="F4:F6" si="1">(D4-D3)/E4*60</f>
         <v>22.028985507246379</v>
       </c>
     </row>
@@ -3084,6 +3117,30 @@
       <c r="F5" s="9">
         <f t="shared" si="1"/>
         <v>10.099009900990099</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="7">
+        <v>43070</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="D6">
+        <f>SUM(Sprint4!G:G)</f>
+        <v>152</v>
+      </c>
+      <c r="E6">
+        <f>SUM(Sprint4!H:H)</f>
+        <v>145</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="1"/>
+        <v>-21.103448275862068</v>
       </c>
     </row>
   </sheetData>
@@ -3098,8 +3155,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:I231"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11:B24"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4411,8 +4468,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2:C9"/>
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B14" sqref="B14:B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4730,10 +4787,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
-  <dimension ref="A1:I9"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="B21" sqref="B21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4780,11 +4837,23 @@
       <c r="C2" t="s">
         <v>176</v>
       </c>
+      <c r="D2" t="s">
+        <v>198</v>
+      </c>
       <c r="E2">
         <v>25</v>
       </c>
       <c r="F2">
         <v>5</v>
+      </c>
+      <c r="G2">
+        <v>25</v>
+      </c>
+      <c r="H2">
+        <v>21</v>
+      </c>
+      <c r="I2" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -4797,11 +4866,23 @@
       <c r="C3" t="s">
         <v>177</v>
       </c>
+      <c r="D3" t="s">
+        <v>198</v>
+      </c>
       <c r="E3">
         <v>10</v>
       </c>
       <c r="F3">
         <v>20</v>
+      </c>
+      <c r="G3">
+        <v>32</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
@@ -4814,11 +4895,23 @@
       <c r="C4" t="s">
         <v>178</v>
       </c>
+      <c r="D4" t="s">
+        <v>198</v>
+      </c>
       <c r="E4">
         <v>45</v>
       </c>
       <c r="F4">
         <v>30</v>
+      </c>
+      <c r="G4">
+        <v>7</v>
+      </c>
+      <c r="H4">
+        <v>3</v>
+      </c>
+      <c r="I4" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
@@ -4860,11 +4953,23 @@
       <c r="C6" t="s">
         <v>176</v>
       </c>
+      <c r="D6" t="s">
+        <v>198</v>
+      </c>
       <c r="E6">
         <v>15</v>
       </c>
       <c r="F6">
         <v>40</v>
+      </c>
+      <c r="G6">
+        <v>15</v>
+      </c>
+      <c r="H6">
+        <v>18</v>
+      </c>
+      <c r="I6" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -4877,11 +4982,23 @@
       <c r="C7" t="s">
         <v>177</v>
       </c>
+      <c r="D7" t="s">
+        <v>198</v>
+      </c>
       <c r="E7">
         <v>50</v>
       </c>
       <c r="F7">
         <v>10</v>
+      </c>
+      <c r="G7">
+        <v>20</v>
+      </c>
+      <c r="H7">
+        <v>15</v>
+      </c>
+      <c r="I7" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
@@ -4894,11 +5011,23 @@
       <c r="C8" t="s">
         <v>178</v>
       </c>
+      <c r="D8" t="s">
+        <v>198</v>
+      </c>
       <c r="E8">
         <v>10</v>
       </c>
       <c r="F8">
         <v>10</v>
+      </c>
+      <c r="G8">
+        <v>12</v>
+      </c>
+      <c r="H8">
+        <v>8</v>
+      </c>
+      <c r="I8" s="13">
+        <v>43070</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
@@ -4929,6 +5058,55 @@
       <c r="I9" s="13">
         <v>43070</v>
       </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="22"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B15" s="21" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B16" s="21" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B17" s="21" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B18" s="21"/>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B19" s="22" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B20" s="21" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B21" s="21" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.2">
+      <c r="B22" s="21"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
@@ -5256,7 +5434,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4" ht="31.5" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>140</v>
       </c>

</xml_diff>